<commit_message>
daily work from omen
</commit_message>
<xml_diff>
--- a/PrototypeLogs/bin/Debug/Logs/Excel.xlsx
+++ b/PrototypeLogs/bin/Debug/Logs/Excel.xlsx
@@ -1,5 +1,12 @@
 
-<file path=xl/workbook.xml>
+<file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
+<x:workbook xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <x:sheets>
+    <x:sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Log" sheetId="1" r:id="Reafb124c71374dd4"/>
+    <x:sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Event" sheetId="2" r:id="R29425a0701964d64"/>
+    <x:sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="PID" sheetId="3" r:id="R640e9c69d0814983"/>
+  </x:sheets>
+</x:workbook>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
@@ -62,7 +69,146 @@
   <x:cols>
     <x:col min="1" max="255" width="19" customWidth="1"/>
   </x:cols>
-  <x:sheetData/>
+  <x:sheetData>
+    <x:row r="1">
+      <x:c s="2" t="str">
+        <x:v>Number</x:v>
+      </x:c>
+      <x:c s="2" t="str">
+        <x:v>Value</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="3">
+      <x:c s="2" t="str">
+        <x:v>20.07.2022 10:14:11:416 7.0.0.16 [1] (INFO): Initializing TCU proxy on port: Simulator for device: TCU. </x:v>
+      </x:c>
+    </x:row>
+    <x:row r="4">
+      <x:c s="2" t="str">
+        <x:v/>
+      </x:c>
+    </x:row>
+    <x:row r="5">
+      <x:c s="2" t="str">
+        <x:v>20.07.2022 10:14:11:621 7.0.0.16 [1] (WARN): TCU device has connected to Simulator port. </x:v>
+      </x:c>
+    </x:row>
+    <x:row r="6">
+      <x:c s="2" t="str">
+        <x:v/>
+      </x:c>
+    </x:row>
+    <x:row r="7">
+      <x:c s="2" t="str">
+        <x:v>20.07.2022 10:14:11:621 7.0.0.16 [19] (WARN): Send Command:GetActiveThermode Token:2 </x:v>
+      </x:c>
+    </x:row>
+    <x:row r="8">
+      <x:c s="2" t="str">
+        <x:v> Response: Not received. </x:v>
+      </x:c>
+    </x:row>
+    <x:row r="9">
+      <x:c s="2" t="str">
+        <x:v/>
+      </x:c>
+    </x:row>
+    <x:row r="10">
+      <x:c s="2" t="str">
+        <x:v>20.07.2022 10:14:11:659 7.0.0.16 [19] (WARN): Send Command:GetThermodeState Token:5  Thermode:TSA</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="11">
+      <x:c s="2" t="str">
+        <x:v> Response: Not received. </x:v>
+      </x:c>
+    </x:row>
+    <x:row r="12">
+      <x:c s="2" t="str">
+        <x:v/>
+      </x:c>
+    </x:row>
+    <x:row r="13">
+      <x:c s="2" t="str">
+        <x:v>20.07.2022 10:14:11:659 7.0.0.16 [19] (WARN): Send Command:GetThermodeState Token:6  Thermode:CHEPS</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="14">
+      <x:c s="2" t="str">
+        <x:v> Response: Not received. </x:v>
+      </x:c>
+    </x:row>
+    <x:row r="15">
+      <x:c s="2" t="str">
+        <x:v/>
+      </x:c>
+    </x:row>
+    <x:row r="16">
+      <x:c s="2" t="str">
+        <x:v>20.07.2022 10:14:11:672 7.0.0.16 [19] (WARN): Send Command:GetThermodeState Token:7  Thermode:CHEPS</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="17">
+      <x:c s="2" t="str">
+        <x:v> Response: Not received. </x:v>
+      </x:c>
+    </x:row>
+    <x:row r="18">
+      <x:c s="2" t="str">
+        <x:v/>
+      </x:c>
+    </x:row>
+    <x:row r="19">
+      <x:c s="2" t="str">
+        <x:v>20.07.2022 10:14:13:203 7.0.0.16 [19] (WARN): Send Command:GetThermodeState Token:38  Thermode:CHEPS</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="20">
+      <x:c s="2" t="str">
+        <x:v> Response: Not received. </x:v>
+      </x:c>
+    </x:row>
+    <x:row r="21">
+      <x:c s="2" t="str">
+        <x:v/>
+      </x:c>
+    </x:row>
+    <x:row r="22">
+      <x:c s="2" t="str">
+        <x:v>20.07.2022 10:14:14:145 7.0.0.16 [19] (WARN): Send Command:SetTcuState Token:57  CommandState:RestMode</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="23">
+      <x:c s="2" t="str">
+        <x:v> Response: Not received. </x:v>
+      </x:c>
+    </x:row>
+    <x:row r="24">
+      <x:c s="2" t="str">
+        <x:v/>
+      </x:c>
+    </x:row>
+    <x:row r="25">
+      <x:c s="2" t="str">
+        <x:v>20.07.2022 10:14:17:146 7.0.0.16 [1] (INFO): START. </x:v>
+      </x:c>
+    </x:row>
+    <x:row r="26">
+      <x:c s="2" t="str">
+        <x:v/>
+      </x:c>
+    </x:row>
+    <x:row r="27">
+      <x:c s="2" t="str">
+        <x:v>20.07.2022 10:14:20:973 7.0.0.16 [1] (INFO): FINISH. </x:v>
+      </x:c>
+    </x:row>
+    <x:row r="28">
+      <x:c s="2" t="str">
+        <x:v/>
+      </x:c>
+    </x:row>
+  </x:sheetData>
 </x:worksheet>
 </file>
 
@@ -73,4 +219,13 @@
   </x:cols>
   <x:sheetData/>
 </x:worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<x:worksheet xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <x:cols>
+    <x:col min="1" max="255" width="25" customWidth="1"/>
+  </x:cols>
+  <x:sheetData/>
+</x:worksheet>
 </file>
</xml_diff>